<commit_message>
addtional amendments to sliders added beginnings of actuarial functions added 92 series xls data
</commit_message>
<xml_diff>
--- a/Mortality_tables/Table_Summary.xlsx
+++ b/Mortality_tables/Table_Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubbe\Google Drive\Actuarial Countryside\Data Visualisation\Mortality Data Dashboard\Python\MDD\Mortality_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2D49CC-4E2B-4DE0-A980-B2240CE53512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5687D42C-3CF6-4129-AA03-228B6CEF639F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8E0869DE-71E2-4B6F-949F-3D79E95B6251}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="133">
   <si>
     <t>AMC00</t>
   </si>
@@ -333,6 +333,108 @@
   </si>
   <si>
     <t>Mortality_tables/HMD_UK_both_sexes_1x1.txt</t>
+  </si>
+  <si>
+    <t>IfoA 92 Series</t>
+  </si>
+  <si>
+    <t>AF92</t>
+  </si>
+  <si>
+    <t>AM92</t>
+  </si>
+  <si>
+    <t>IFA92</t>
+  </si>
+  <si>
+    <t>IFL92</t>
+  </si>
+  <si>
+    <t>IMA92</t>
+  </si>
+  <si>
+    <t>IML92</t>
+  </si>
+  <si>
+    <t>PFA92</t>
+  </si>
+  <si>
+    <t>PFL92</t>
+  </si>
+  <si>
+    <t>PMA92</t>
+  </si>
+  <si>
+    <t>PML92</t>
+  </si>
+  <si>
+    <t>RFV92</t>
+  </si>
+  <si>
+    <t>RMV92</t>
+  </si>
+  <si>
+    <t>TF92</t>
+  </si>
+  <si>
+    <t>TM92</t>
+  </si>
+  <si>
+    <t>WA92</t>
+  </si>
+  <si>
+    <t>WL92</t>
+  </si>
+  <si>
+    <t>AF92: Permanent Assurances, females, combined</t>
+  </si>
+  <si>
+    <t>Mortality_tables/92series.xls</t>
+  </si>
+  <si>
+    <t>AM92: Permanent Assurances, males, combined</t>
+  </si>
+  <si>
+    <t>IFA92: Immediate Annuitants, females, amounts</t>
+  </si>
+  <si>
+    <t>IFA92: Immediate Annuitants, females, lives</t>
+  </si>
+  <si>
+    <t>IMA92: Immediate Annuitants, males, amounts</t>
+  </si>
+  <si>
+    <t>IMA92: Immediate Annuitants, males, lives</t>
+  </si>
+  <si>
+    <t>PFA92: Pensioners, females, amounts</t>
+  </si>
+  <si>
+    <t>PFL92: Pensioners, females, lives</t>
+  </si>
+  <si>
+    <t>PMA92: Pensioners, males, amounts</t>
+  </si>
+  <si>
+    <t>PML92: Pensioners, males, lives</t>
+  </si>
+  <si>
+    <t>RFV92: Retirement Annuitants, females, vested</t>
+  </si>
+  <si>
+    <t>RMV92: Retirement Annuitants, males, vested</t>
+  </si>
+  <si>
+    <t>TF92: Temporary Assurances, females, combined</t>
+  </si>
+  <si>
+    <t>TM92: Temporary Assurances, males, combined</t>
+  </si>
+  <si>
+    <t>WA92: Widows, amounts</t>
+  </si>
+  <si>
+    <t>WL92: Widows, lives</t>
   </si>
 </sst>
 </file>
@@ -685,7 +787,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -694,10 +796,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1AB3AF5-6D31-43A2-80C9-BC1AA1AFEEE5}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="87" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1471,6 +1573,278 @@
         <v>0</v>
       </c>
     </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" t="s">
+        <v>116</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" t="s">
+        <v>118</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" t="s">
+        <v>102</v>
+      </c>
+      <c r="C48" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" t="s">
+        <v>120</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>104</v>
+      </c>
+      <c r="C50" t="s">
+        <v>121</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" t="s">
+        <v>122</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" t="s">
+        <v>124</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" t="s">
+        <v>125</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C55" t="s">
+        <v>126</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" t="s">
+        <v>127</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>99</v>
+      </c>
+      <c r="B58" t="s">
+        <v>112</v>
+      </c>
+      <c r="C58" t="s">
+        <v>129</v>
+      </c>
+      <c r="D58">
+        <v>5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" t="s">
+        <v>130</v>
+      </c>
+      <c r="D59">
+        <v>5</v>
+      </c>
+      <c r="E59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" t="s">
+        <v>114</v>
+      </c>
+      <c r="C60" t="s">
+        <v>131</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>99</v>
+      </c>
+      <c r="B61" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" t="s">
+        <v>132</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>